<commit_message>
remove external libraries and use maven dependency poi ooxml to use workbook and sheet libraries
</commit_message>
<xml_diff>
--- a/target/classes/Fakha.xlsx
+++ b/target/classes/Fakha.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="33">
   <si>
     <t xml:space="preserve">insert</t>
   </si>
@@ -110,10 +110,13 @@
     <t xml:space="preserve">'DObPaymentRequest'</t>
   </si>
   <si>
+    <t xml:space="preserve">alter-sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dobpaymentrequest_id_seq</t>
+  </si>
+  <si>
     <t xml:space="preserve">sequence-restart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dobpaymentrequest_id_seq</t>
   </si>
   <si>
     <t xml:space="preserve">'2019000004'</t>
@@ -126,7 +129,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -148,6 +151,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,12 +203,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -218,22 +233,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.53"/>
@@ -284,37 +299,37 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="I3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="2" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -397,37 +412,37 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="J8" s="0" t="s">
+      <c r="I8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -510,37 +525,37 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="2" t="n">
         <v>1001</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="J13" s="0" t="s">
+      <c r="I13" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="2" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -587,49 +602,49 @@
         <v>1</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>1005</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -651,7 +666,7 @@
   </sheetPr>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -659,14 +674,14 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="22.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="22.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.39"/>
   </cols>
   <sheetData>
@@ -680,7 +695,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>30</v>
@@ -745,7 +760,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>